<commit_message>
[Feat] 나무 NPC 추가
</commit_message>
<xml_diff>
--- a/Assets/Resources/Additional/Excel/BlackSmith.xlsx
+++ b/Assets/Resources/Additional/Excel/BlackSmith.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\unity\Become_Celebrity_on_Farm\Assets\02.Scripts\12.NPC\TextUIManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\unity\Become_Celebrity_on_Farm\Assets\Resources\Additional\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A583C5B-A3C3-4300-B8DD-5D75D4D7C7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D90D864-6161-4ACC-9E61-0EDE82B357AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,13 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>BlackSmith_0</t>
-  </si>
-  <si>
-    <t>BlackSmith_3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Daily</t>
@@ -45,19 +41,23 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>오늘도 왔는가</t>
+  </si>
+  <si>
+    <t>BlackSmith_0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>요즘 농사는 괜찮게 되고 있지?</t>
+  </si>
+  <si>
     <t>좋은 상품이 들어왔는데 보고 가겠나?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>오늘도 왔는가</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>요즘 농사는 괜찮게 되고 있지?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>우리 마을의 유일 마트라고</t>
+  </si>
+  <si>
+    <t>BlackSmith_3</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -381,10 +381,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -393,12 +393,12 @@
     <col min="2" max="2" width="22.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C1">
         <v>0</v>
@@ -407,21 +407,24 @@
         <v>100</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
+      <c r="H1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -430,21 +433,24 @@
         <v>100</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -453,16 +459,19 @@
         <v>100</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -476,14 +485,29 @@
         <v>100</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="G4" t="b">
         <v>0</v>
       </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>